<commit_message>
updates to western and qpcr
</commit_message>
<xml_diff>
--- a/data/tr010_age_participant.xlsx
+++ b/data/tr010_age_participant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\706194\projects\ribo-accum-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CB3D9E-F40C-4246-9599-DC15F1A09DD4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0D30C0-1335-4B70-B857-484244A6387D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30390" yWindow="1320" windowWidth="28500" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +880,7 @@
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="2">
         <v>34265</v>
       </c>
       <c r="D17" s="5">
@@ -906,7 +906,7 @@
       <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="2">
         <v>35323</v>
       </c>
       <c r="D18" s="5">
@@ -932,6 +932,9 @@
       <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="C19" s="2">
+        <v>35733</v>
+      </c>
       <c r="D19" s="5">
         <v>43756</v>
       </c>
@@ -955,7 +958,7 @@
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="2">
         <v>30860</v>
       </c>
       <c r="D20" s="5">

</xml_diff>

<commit_message>
sorted files and added manual edits
</commit_message>
<xml_diff>
--- a/data/tr010_age_participant.xlsx
+++ b/data/tr010_age_participant.xlsx
@@ -5,27 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\706194\projects\ribo-accum-paper\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\706194\Dropbox\1. Research\1. phd\phd PROJECTS\6. Ribosome accumulation\ribo-accum-paper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393A4DA4-C280-4663-B39E-176363F04A4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EBDE88-F6E4-4633-AFF1-06BB2396FA46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33015" yWindow="1785" windowWidth="17430" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8820" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
   <si>
     <t>P1</t>
   </si>
@@ -72,12 +78,6 @@
     <t>P15</t>
   </si>
   <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>recruited</t>
-  </si>
-  <si>
     <t>group</t>
   </si>
   <si>
@@ -124,16 +124,27 @@
   </si>
   <si>
     <t>P23</t>
+  </si>
+  <si>
+    <t>age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,18 +170,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,536 +461,476 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
       </c>
       <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2">
-        <v>35231</v>
-      </c>
-      <c r="D2" s="2">
-        <v>43105</v>
+        <v>16</v>
+      </c>
+      <c r="C2" s="4">
+        <v>21.558279773027508</v>
+      </c>
+      <c r="D2">
+        <v>172</v>
       </c>
       <c r="E2">
-        <v>172</v>
-      </c>
-      <c r="F2">
         <v>63.8</v>
       </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
       <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2">
-        <v>35847</v>
-      </c>
-      <c r="D3" s="2">
-        <v>43105</v>
+        <v>16</v>
+      </c>
+      <c r="C3" s="4">
+        <v>19.871729056722589</v>
+      </c>
+      <c r="D3">
+        <v>180</v>
       </c>
       <c r="E3">
-        <v>180</v>
-      </c>
-      <c r="F3">
         <v>81.2</v>
       </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2">
-        <v>35313</v>
-      </c>
-      <c r="D4" s="2">
-        <v>43103</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>21.328295584440475</v>
+      </c>
+      <c r="D4">
+        <v>164</v>
       </c>
       <c r="E4">
-        <v>164</v>
-      </c>
-      <c r="F4">
         <v>59</v>
       </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
       <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2">
-        <v>33968</v>
-      </c>
-      <c r="D5" s="2">
-        <v>43108</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="4">
+        <v>25.02447004387496</v>
+      </c>
+      <c r="D5">
+        <v>177</v>
       </c>
       <c r="E5">
-        <v>177</v>
-      </c>
-      <c r="F5">
         <v>66.5</v>
       </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2">
-        <v>33899</v>
-      </c>
-      <c r="D6" s="2">
-        <v>43108</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="4">
+        <v>25.213385627357166</v>
+      </c>
+      <c r="D6">
+        <v>174</v>
       </c>
       <c r="E6">
-        <v>174</v>
-      </c>
-      <c r="F6">
         <v>72.7</v>
       </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2">
-        <v>35232</v>
-      </c>
-      <c r="D7" s="2">
-        <v>43122</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="4">
+        <v>21.602086285139325</v>
+      </c>
+      <c r="D7">
+        <v>171</v>
       </c>
       <c r="E7">
-        <v>171</v>
-      </c>
-      <c r="F7">
         <v>55.2</v>
       </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
       <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2">
-        <v>32901</v>
-      </c>
-      <c r="D8" s="2">
-        <v>43133</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <v>28.01426449550641</v>
+      </c>
+      <c r="D8">
+        <v>180</v>
       </c>
       <c r="E8">
-        <v>180</v>
-      </c>
-      <c r="F8">
         <v>81.3</v>
       </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2">
-        <v>35270</v>
-      </c>
-      <c r="D9" s="2">
-        <v>43116</v>
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <v>21.481618376831829</v>
+      </c>
+      <c r="D9">
+        <v>185</v>
       </c>
       <c r="E9">
-        <v>185</v>
-      </c>
-      <c r="F9">
         <v>75.5</v>
       </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="2">
-        <v>33465</v>
-      </c>
-      <c r="D10" s="2">
-        <v>43119</v>
+        <v>17</v>
+      </c>
+      <c r="C10" s="4">
+        <v>26.431754245467051</v>
+      </c>
+      <c r="D10">
+        <v>171</v>
       </c>
       <c r="E10">
-        <v>171</v>
-      </c>
-      <c r="F10">
         <v>63.7</v>
       </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
       <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2">
-        <v>35901</v>
-      </c>
-      <c r="D11" s="2">
-        <v>43126</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="4">
+        <v>19.781378125491969</v>
+      </c>
+      <c r="D11">
+        <v>162</v>
       </c>
       <c r="E11">
-        <v>162</v>
-      </c>
-      <c r="F11">
         <v>64</v>
       </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="2">
-        <v>34718</v>
-      </c>
-      <c r="D12" s="2">
-        <v>43146</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="4">
+        <v>23.075080254899142</v>
+      </c>
+      <c r="D12">
+        <v>186</v>
       </c>
       <c r="E12">
-        <v>186</v>
-      </c>
-      <c r="F12">
         <v>75.900000000000006</v>
       </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
       <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="H12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2">
-        <v>34511</v>
-      </c>
-      <c r="D13" s="2">
-        <v>43151</v>
+        <v>17</v>
+      </c>
+      <c r="C13" s="4">
+        <v>23.655516540380706</v>
+      </c>
+      <c r="D13">
+        <v>181</v>
       </c>
       <c r="E13">
-        <v>181</v>
-      </c>
-      <c r="F13">
         <v>67.8</v>
       </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
       <c r="G13" t="s">
         <v>24</v>
       </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2">
-        <v>30860</v>
-      </c>
-      <c r="D14" s="2">
-        <v>43151</v>
-      </c>
-      <c r="E14" s="1">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4">
+        <v>33.651615022895747</v>
+      </c>
+      <c r="D14" s="1">
         <v>175</v>
       </c>
-      <c r="F14">
+      <c r="E14">
         <v>85</v>
       </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
       <c r="G14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="2">
-        <v>34864</v>
-      </c>
-      <c r="D15" s="2">
-        <v>43157</v>
-      </c>
-      <c r="E15" s="1">
+        <v>17</v>
+      </c>
+      <c r="C15" s="4">
+        <v>22.705462808955694</v>
+      </c>
+      <c r="D15" s="1">
         <v>165</v>
       </c>
-      <c r="F15">
+      <c r="E15">
         <v>64.2</v>
       </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
       <c r="G15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="4">
+        <v>27.485848443157629</v>
+      </c>
+      <c r="D16" s="1">
+        <v>166</v>
+      </c>
+      <c r="E16">
+        <v>63</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="4">
+        <v>26.001902845369855</v>
+      </c>
+      <c r="D17" s="1">
+        <v>163</v>
+      </c>
+      <c r="E17">
+        <v>60</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4">
-        <v>33708</v>
-      </c>
-      <c r="D16" s="5">
-        <v>43747</v>
-      </c>
-      <c r="E16" s="1">
-        <v>166</v>
-      </c>
-      <c r="F16">
-        <v>63</v>
-      </c>
-      <c r="G16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4">
+        <v>23.096983510955049</v>
+      </c>
+      <c r="D18" s="1">
+        <v>181</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="2">
-        <v>34265</v>
-      </c>
-      <c r="D17" s="5">
-        <v>43762</v>
-      </c>
-      <c r="E17" s="1">
-        <v>163</v>
-      </c>
-      <c r="F17">
-        <v>60</v>
-      </c>
-      <c r="G17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4">
+        <v>21.966227917068796</v>
+      </c>
+      <c r="D19" s="1">
+        <v>157</v>
+      </c>
+      <c r="E19">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="2">
-        <v>35323</v>
-      </c>
-      <c r="D18" s="5">
-        <v>43759</v>
-      </c>
-      <c r="E18" s="1">
-        <v>181</v>
-      </c>
-      <c r="F18">
-        <v>80</v>
-      </c>
-      <c r="G18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2">
-        <v>35733</v>
-      </c>
-      <c r="D19" s="5">
-        <v>43756</v>
-      </c>
-      <c r="E19" s="1">
-        <v>157</v>
-      </c>
-      <c r="F19">
-        <v>65</v>
-      </c>
-      <c r="G19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2">
-        <v>30860</v>
-      </c>
-      <c r="D20" s="5">
-        <v>43756</v>
-      </c>
-      <c r="E20" s="1">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4">
+        <v>35.308048762123796</v>
+      </c>
+      <c r="D20" s="1">
         <v>174</v>
       </c>
-      <c r="F20">
+      <c r="E20">
         <v>87</v>
       </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
       <c r="G20" t="s">
         <v>24</v>
       </c>
-      <c r="H20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="1048576" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E1048576" s="1"/>
+    </row>
+    <row r="1048576" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1048576" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>